<commit_message>
file input: fast reading binary
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>N потоков</t>
+  </si>
+  <si>
+    <t>t read file</t>
   </si>
   <si>
     <t>t der, s</t>
@@ -35,6 +38,39 @@
   </si>
   <si>
     <t>t only der_1, s</t>
+  </si>
+  <si>
+    <t>lines</t>
+  </si>
+  <si>
+    <t>speed [lines / s]</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>speed [points / s]</t>
+  </si>
+  <si>
+    <t>N array</t>
+  </si>
+  <si>
+    <t>push_back</t>
+  </si>
+  <si>
+    <t>no push_back</t>
+  </si>
+  <si>
+    <t>ram</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>hdd</t>
+  </si>
+  <si>
+    <t>ssd</t>
   </si>
 </sst>
 </file>
@@ -70,8 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -531,7 +571,364 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no push_back</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$26:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$26:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="413224944"/>
+        <c:axId val="460113064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="413224944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="460113064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="460113064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413224944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1087,6 +1484,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1114,6 +2027,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1409,10 +2352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,22 +2374,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1582,8 +2525,472 @@
         <v>10</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.5679999999999996</v>
+      </c>
+      <c r="B15">
+        <f>1000*1700</f>
+        <v>1700000</v>
+      </c>
+      <c r="C15" s="1">
+        <f>B15/A15</f>
+        <v>258830.69427527406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>18.751000000000001</v>
+      </c>
+      <c r="C20">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D20" s="1">
+        <f>C20/B20</f>
+        <v>2666524.452029225</v>
+      </c>
+      <c r="E20">
+        <f>C20*8/(1024*1024)</f>
+        <v>381.4697265625</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>16.052</v>
+      </c>
+      <c r="C21">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D21" s="1">
+        <f>C21/B21</f>
+        <v>3114876.650884625</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>15.696</v>
+      </c>
+      <c r="C22">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D22" s="1">
+        <f>C22/B22</f>
+        <v>3185524.9745158004</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1000</v>
+      </c>
+      <c r="B23">
+        <v>15.631</v>
+      </c>
+      <c r="C23">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D23" s="1">
+        <f>C23/B23</f>
+        <v>3198771.6716780756</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>3.23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>100</v>
+      </c>
+      <c r="B28">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B30">
+        <v>0.11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B31">
+        <v>0.11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>3.1040000000000001</v>
+      </c>
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <v>0.219</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B36">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B37">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B38">
+        <v>0.109</v>
+      </c>
+      <c r="F38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>3.1360000000000001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>100</v>
+      </c>
+      <c r="B42">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B43">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B44">
+        <v>0.125</v>
+      </c>
+      <c r="F44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B45">
+        <v>9.4E-2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>4.29</v>
+      </c>
+      <c r="C49">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D49" s="1">
+        <f>C49/B49</f>
+        <v>11655011.655011656</v>
+      </c>
+      <c r="E49">
+        <f>C49*8/(1024*1024)</f>
+        <v>381.4697265625</v>
+      </c>
+      <c r="F49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="C50">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D50" s="1">
+        <f>C50/B50</f>
+        <v>82236842.105263159</v>
+      </c>
+      <c r="F50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>100</v>
+      </c>
+      <c r="B51">
+        <v>0.375</v>
+      </c>
+      <c r="C51">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D51" s="1">
+        <f>C51/B51</f>
+        <v>133333333.33333333</v>
+      </c>
+      <c r="F51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1000</v>
+      </c>
+      <c r="B52">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="C52">
+        <f>50*1000*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="D52" s="1">
+        <f>C52/B52</f>
+        <v>86505190.311418697</v>
+      </c>
+      <c r="F52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10000</v>
+      </c>
+      <c r="B53">
+        <v>0.218</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>100000</v>
+      </c>
+      <c r="B54">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B25:E25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MPI parser: 1 core
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>N потоков</t>
   </si>
@@ -71,6 +72,15 @@
   </si>
   <si>
     <t>ssd</t>
+  </si>
+  <si>
+    <t>N proseces</t>
+  </si>
+  <si>
+    <t>t, s</t>
+  </si>
+  <si>
+    <t>speedup</t>
   </si>
 </sst>
 </file>
@@ -888,6 +898,446 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>theory</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист2!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист2!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>real</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист2!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист2!$J$2:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1746540235776526</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9868004223864832</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6638601036269431</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4403453689167973</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8599656357388312</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3671726755218225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6797188755020072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3848758465011288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1983199415631844</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2522104332449162</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7685248130523457</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="466756160"/>
+        <c:axId val="466755768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="466756160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="466755768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="466755768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="466756160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -968,6 +1418,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1485,6 +1975,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2057,6 +3063,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2354,7 +3395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2993,4 +4034,226 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>35.159999999999997</v>
+      </c>
+      <c r="C2">
+        <v>26.28</v>
+      </c>
+      <c r="D2">
+        <v>25.9</v>
+      </c>
+      <c r="E2">
+        <v>25.8</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE($B$2:$H$2)/AVERAGE(B2:H2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>13.12</v>
+      </c>
+      <c r="D3">
+        <v>12.9</v>
+      </c>
+      <c r="J3">
+        <f>AVERAGE($B$2:$H$2)/AVERAGE(B3:H3)</f>
+        <v>2.1746540235776526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J13" si="0">AVERAGE($B$2:$H$2)/AVERAGE(B4:H4)</f>
+        <v>2.9868004223864832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>7.72</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>3.6638601036269431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6.37</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>4.4403453689167973</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5.82</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>4.8599656357388312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5.27</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>5.3671726755218225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>5.6797188755020072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4.43</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>6.3848758465011288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>5.9</v>
+      </c>
+      <c r="C11">
+        <v>5.51</v>
+      </c>
+      <c r="D11">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E11">
+        <v>3.98</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>3.97</v>
+      </c>
+      <c r="J11">
+        <f>AVERAGE($B$2:$H$2)/AVERAGE(B11:H11)</f>
+        <v>6.1983199415631844</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>5.21</v>
+      </c>
+      <c r="C12">
+        <v>3.6</v>
+      </c>
+      <c r="D12">
+        <v>3.64</v>
+      </c>
+      <c r="E12">
+        <v>4.99</v>
+      </c>
+      <c r="F12">
+        <v>5.18</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>6.2522104332449162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5.2</v>
+      </c>
+      <c r="C13">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D13">
+        <v>4.82</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>5.7685248130523457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>